<commit_message>
Lab01 -> using reflections lib added
</commit_message>
<xml_diff>
--- a/Lab01/SortStatistics.xlsx
+++ b/Lab01/SortStatistics.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="9">
   <si>
     <t>size</t>
   </si>
@@ -4231,64 +4231,64 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0184698</v>
+        <v>0.0188522</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0364752</v>
+        <v>0.048637</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0291843</v>
+        <v>0.0294896</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0254887</v>
+        <v>0.0276752</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0427268</v>
+        <v>0.0435326</v>
       </c>
       <c r="G2" t="n">
-        <v>0.063917</v>
+        <v>0.0648922</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0893827</v>
+        <v>0.0929396</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1225319</v>
+        <v>0.1237894</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1546803</v>
+        <v>0.1553732</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1953797</v>
+        <v>0.1923489</v>
       </c>
       <c r="L2" t="n">
-        <v>0.2433855</v>
+        <v>0.2343392</v>
       </c>
       <c r="M2" t="n">
-        <v>0.2896666</v>
+        <v>0.3324114</v>
       </c>
       <c r="N2" t="n">
-        <v>0.3350394</v>
+        <v>0.3464878</v>
       </c>
       <c r="O2" t="n">
-        <v>0.3906722</v>
+        <v>0.3892069</v>
       </c>
       <c r="P2" t="n">
-        <v>0.4494951</v>
+        <v>0.4491307</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.5184216</v>
+        <v>0.5160067</v>
       </c>
       <c r="R2" t="n">
-        <v>0.5922497</v>
+        <v>0.586129</v>
       </c>
       <c r="S2" t="n">
-        <v>0.6560256</v>
+        <v>0.6567108</v>
       </c>
       <c r="T2" t="n">
-        <v>0.7430447</v>
+        <v>0.7435297</v>
       </c>
       <c r="U2" t="n">
-        <v>0.8147813</v>
+        <v>0.8175914</v>
       </c>
     </row>
     <row r="3">
@@ -4296,259 +4296,259 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0117229</v>
+        <v>0.0059128</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0328541</v>
+        <v>0.0333751</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0162782</v>
+        <v>0.0244802</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0250294</v>
+        <v>0.0264716</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0423803</v>
+        <v>0.0429603</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0636731</v>
+        <v>0.066355</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0890798</v>
+        <v>0.0916821</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1203839</v>
+        <v>0.1199733</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1535845</v>
+        <v>0.1553065</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1923181</v>
+        <v>0.1932061</v>
       </c>
       <c r="L3" t="n">
-        <v>0.234814</v>
+        <v>0.2534198</v>
       </c>
       <c r="M3" t="n">
-        <v>0.2824707</v>
+        <v>0.282386</v>
       </c>
       <c r="N3" t="n">
-        <v>0.3328375</v>
+        <v>0.3348392</v>
       </c>
       <c r="O3" t="n">
-        <v>0.3896714</v>
+        <v>0.3897304</v>
       </c>
       <c r="P3" t="n">
-        <v>0.4542095</v>
+        <v>0.4487509</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.5144386</v>
+        <v>0.5175336</v>
       </c>
       <c r="R3" t="n">
-        <v>0.5813659</v>
+        <v>0.5834318</v>
       </c>
       <c r="S3" t="n">
-        <v>0.6572241</v>
+        <v>0.6641891</v>
       </c>
       <c r="T3" t="n">
-        <v>0.7344424</v>
+        <v>0.7398573</v>
       </c>
       <c r="U3" t="n">
-        <v>0.8188156</v>
+        <v>0.8253494</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>4.465E-4</v>
+        <v>0.0067083</v>
       </c>
       <c r="C4" t="n">
-        <v>0.001047</v>
+        <v>0.0059872</v>
       </c>
       <c r="D4" t="n">
-        <v>0.001822</v>
+        <v>0.0064286</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0025252</v>
+        <v>0.0095595</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0032643</v>
+        <v>0.0123722</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0041061</v>
+        <v>0.0157983</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0039803</v>
+        <v>0.0182132</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0020684</v>
+        <v>0.0214442</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0018477</v>
+        <v>0.0170045</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0020556</v>
+        <v>0.0143047</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0022866</v>
+        <v>0.0145741</v>
       </c>
       <c r="M4" t="n">
-        <v>0.002497</v>
+        <v>0.0159625</v>
       </c>
       <c r="N4" t="n">
-        <v>0.0027152</v>
+        <v>0.0169762</v>
       </c>
       <c r="O4" t="n">
-        <v>0.0033849</v>
+        <v>0.0211183</v>
       </c>
       <c r="P4" t="n">
-        <v>0.0031386</v>
+        <v>0.0212441</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.0036698</v>
+        <v>0.0228454</v>
       </c>
       <c r="R4" t="n">
-        <v>0.0051814</v>
+        <v>0.0294845</v>
       </c>
       <c r="S4" t="n">
-        <v>0.0056561</v>
+        <v>0.0228429</v>
       </c>
       <c r="T4" t="n">
-        <v>0.0057922</v>
+        <v>0.0196093</v>
       </c>
       <c r="U4" t="n">
-        <v>0.0013319</v>
+        <v>0.0216803</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0058332</v>
+        <v>4.824E-4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0052635</v>
+        <v>0.0016527</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0069496</v>
+        <v>0.0028948</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0096186</v>
+        <v>0.0041163</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0126442</v>
+        <v>0.005456</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0089693</v>
+        <v>0.0067032</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0074089</v>
+        <v>0.0079941</v>
       </c>
       <c r="I5" t="n">
-        <v>0.008728</v>
+        <v>0.0092285</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0096802</v>
+        <v>0.0106554</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0114355</v>
+        <v>0.0118204</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0127084</v>
+        <v>0.0130934</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0136451</v>
+        <v>0.0143817</v>
       </c>
       <c r="N5" t="n">
-        <v>0.0147512</v>
+        <v>0.0158983</v>
       </c>
       <c r="O5" t="n">
-        <v>0.0255786</v>
+        <v>0.0170737</v>
       </c>
       <c r="P5" t="n">
-        <v>0.0214288</v>
+        <v>0.0184904</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.0185802</v>
+        <v>0.0196683</v>
       </c>
       <c r="R5" t="n">
-        <v>0.0194784</v>
+        <v>0.0210079</v>
       </c>
       <c r="S5" t="n">
-        <v>0.0257454</v>
+        <v>0.0222757</v>
       </c>
       <c r="T5" t="n">
-        <v>0.0159292</v>
+        <v>0.0236846</v>
       </c>
       <c r="U5" t="n">
-        <v>0.0167427</v>
+        <v>0.0250088</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0148641</v>
+        <v>9.803E-4</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0060539</v>
+        <v>0.0013986</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0127957</v>
+        <v>0.0026048</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0173458</v>
+        <v>0.0017374</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0166554</v>
+        <v>0.0014474</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0079043</v>
+        <v>0.0018452</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0082456</v>
+        <v>0.0023122</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0117769</v>
+        <v>0.0021095</v>
       </c>
       <c r="J6" t="n">
-        <v>0.016137</v>
+        <v>0.0018272</v>
       </c>
       <c r="K6" t="n">
-        <v>0.0178822</v>
+        <v>0.0025637</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0200789</v>
+        <v>0.00329</v>
       </c>
       <c r="M6" t="n">
-        <v>0.016853</v>
+        <v>0.0037879</v>
       </c>
       <c r="N6" t="n">
-        <v>0.0160729</v>
+        <v>0.004296</v>
       </c>
       <c r="O6" t="n">
-        <v>0.0172662</v>
+        <v>0.0042678</v>
       </c>
       <c r="P6" t="n">
-        <v>0.0182543</v>
+        <v>0.0047502</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.0202098</v>
+        <v>0.003544</v>
       </c>
       <c r="R6" t="n">
-        <v>0.020972</v>
+        <v>9.777E-4</v>
       </c>
       <c r="S6" t="n">
-        <v>0.0225606</v>
+        <v>0.001047</v>
       </c>
       <c r="T6" t="n">
-        <v>0.0234151</v>
+        <v>0.001106</v>
       </c>
       <c r="U6" t="n">
-        <v>0.0268207</v>
+        <v>0.0011702</v>
       </c>
     </row>
   </sheetData>
@@ -4632,64 +4632,64 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0035569</v>
+        <v>6.672E-4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0137298</v>
+        <v>0.0081044</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0204998</v>
+        <v>0.0213724</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0258557</v>
+        <v>0.039329</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0427524</v>
+        <v>0.0652361</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0638246</v>
+        <v>0.0664627</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0904708</v>
+        <v>0.0922082</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1294225</v>
+        <v>0.1433012</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1579344</v>
+        <v>0.1536204</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1908784</v>
+        <v>0.261722</v>
       </c>
       <c r="L2" t="n">
-        <v>0.2347729</v>
+        <v>0.2449972</v>
       </c>
       <c r="M2" t="n">
-        <v>0.2810079</v>
+        <v>0.2838</v>
       </c>
       <c r="N2" t="n">
-        <v>0.3355757</v>
+        <v>0.337444</v>
       </c>
       <c r="O2" t="n">
-        <v>0.3970162</v>
+        <v>0.3893891</v>
       </c>
       <c r="P2" t="n">
-        <v>0.4625321</v>
+        <v>0.4490639</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.5242625</v>
+        <v>0.5140973</v>
       </c>
       <c r="R2" t="n">
-        <v>0.5925988</v>
+        <v>0.5930889</v>
       </c>
       <c r="S2" t="n">
-        <v>0.6561282</v>
+        <v>0.6686802</v>
       </c>
       <c r="T2" t="n">
-        <v>0.7306775</v>
+        <v>0.7485212</v>
       </c>
       <c r="U2" t="n">
-        <v>0.819606</v>
+        <v>0.827459</v>
       </c>
     </row>
     <row r="3">
@@ -4697,259 +4697,259 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0036441</v>
+        <v>4.722E-4</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0283707</v>
+        <v>0.0046861</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0197068</v>
+        <v>0.013445</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0253065</v>
+        <v>0.0262022</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0425035</v>
+        <v>0.0426421</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0634345</v>
+        <v>0.0658391</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0891132</v>
+        <v>0.0894211</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1200092</v>
+        <v>0.1235225</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1531662</v>
+        <v>0.1532073</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1919871</v>
+        <v>0.1968733</v>
       </c>
       <c r="L3" t="n">
-        <v>0.2343135</v>
+        <v>0.2419894</v>
       </c>
       <c r="M3" t="n">
-        <v>0.281942</v>
+        <v>0.288055</v>
       </c>
       <c r="N3" t="n">
-        <v>0.3342952</v>
+        <v>0.3331429</v>
       </c>
       <c r="O3" t="n">
-        <v>0.3879109</v>
+        <v>0.3897638</v>
       </c>
       <c r="P3" t="n">
-        <v>0.4510375</v>
+        <v>0.4534858</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.5122085</v>
+        <v>0.5209905</v>
       </c>
       <c r="R3" t="n">
-        <v>0.584928</v>
+        <v>0.5826645</v>
       </c>
       <c r="S3" t="n">
-        <v>0.6533361</v>
+        <v>0.6626082</v>
       </c>
       <c r="T3" t="n">
-        <v>0.7327075</v>
+        <v>0.7343756</v>
       </c>
       <c r="U3" t="n">
-        <v>0.8258961</v>
+        <v>0.8266634</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0013396</v>
+        <v>3.798E-4</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0016732</v>
+        <v>0.0012831</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0035312</v>
+        <v>0.002325</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0016629</v>
+        <v>0.0034363</v>
       </c>
       <c r="F4" t="n">
-        <v>0.002284</v>
+        <v>0.0043807</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0018451</v>
+        <v>0.00561</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0022198</v>
+        <v>0.0067186</v>
       </c>
       <c r="I4" t="n">
-        <v>0.002438</v>
+        <v>0.0081917</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0027536</v>
+        <v>0.0111763</v>
       </c>
       <c r="K4" t="n">
-        <v>0.003195</v>
+        <v>0.0102319</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0038007</v>
+        <v>0.0108555</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0049145</v>
+        <v>0.012113</v>
       </c>
       <c r="N4" t="n">
-        <v>0.013581</v>
+        <v>0.0130857</v>
       </c>
       <c r="O4" t="n">
-        <v>0.002515</v>
+        <v>0.0147589</v>
       </c>
       <c r="P4" t="n">
-        <v>0.0012883</v>
+        <v>0.0156315</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.0013858</v>
+        <v>0.0177128</v>
       </c>
       <c r="R4" t="n">
-        <v>0.0015346</v>
+        <v>0.0183518</v>
       </c>
       <c r="S4" t="n">
-        <v>0.0015783</v>
+        <v>0.0192166</v>
       </c>
       <c r="T4" t="n">
-        <v>0.0016706</v>
+        <v>0.0200763</v>
       </c>
       <c r="U4" t="n">
-        <v>0.0017527</v>
+        <v>0.0216726</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0053969</v>
+        <v>5.26E-4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0083739</v>
+        <v>0.0016604</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0116023</v>
+        <v>0.0029256</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0160241</v>
+        <v>0.0041702</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0209899</v>
+        <v>0.0054662</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0199147</v>
+        <v>0.0067853</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0147974</v>
+        <v>0.0082045</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0176409</v>
+        <v>0.009385</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0143996</v>
+        <v>0.0110737</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0123055</v>
+        <v>0.0119206</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0160267</v>
+        <v>0.0138504</v>
       </c>
       <c r="M5" t="n">
-        <v>0.015054</v>
+        <v>0.0146768</v>
       </c>
       <c r="N5" t="n">
-        <v>0.0159343</v>
+        <v>0.0165656</v>
       </c>
       <c r="O5" t="n">
-        <v>0.0183826</v>
+        <v>0.0175562</v>
       </c>
       <c r="P5" t="n">
-        <v>0.0192089</v>
+        <v>0.0186366</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.0207256</v>
+        <v>0.0201277</v>
       </c>
       <c r="R5" t="n">
-        <v>0.0211055</v>
+        <v>0.0213261</v>
       </c>
       <c r="S5" t="n">
-        <v>0.02254</v>
+        <v>0.0227736</v>
       </c>
       <c r="T5" t="n">
-        <v>0.0180643</v>
+        <v>0.024244</v>
       </c>
       <c r="U5" t="n">
-        <v>0.0199326</v>
+        <v>0.0255324</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>4.85E-4</v>
+        <v>3.33E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.001627</v>
+        <v>9.23E-5</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0028511</v>
+        <v>1.642E-4</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0041292</v>
+        <v>2.566E-4</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0053841</v>
+        <v>3.438E-4</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0066467</v>
+        <v>4.439E-4</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0078657</v>
+        <v>5.132E-4</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0092336</v>
+        <v>6.056E-4</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0104578</v>
+        <v>6.954E-4</v>
       </c>
       <c r="K6" t="n">
-        <v>0.0117897</v>
+        <v>7.827E-4</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0133628</v>
+        <v>8.853E-4</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0144381</v>
+        <v>9.777E-4</v>
       </c>
       <c r="N6" t="n">
-        <v>0.0164193</v>
+        <v>0.0010752</v>
       </c>
       <c r="O6" t="n">
-        <v>0.0170558</v>
+        <v>0.0011446</v>
       </c>
       <c r="P6" t="n">
-        <v>0.0190934</v>
+        <v>0.0012215</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.0198787</v>
+        <v>0.0013319</v>
       </c>
       <c r="R6" t="n">
-        <v>0.0208668</v>
+        <v>0.0014037</v>
       </c>
       <c r="S6" t="n">
-        <v>0.0229712</v>
+        <v>0.0015064</v>
       </c>
       <c r="T6" t="n">
-        <v>0.0235768</v>
+        <v>0.0016167</v>
       </c>
       <c r="U6" t="n">
-        <v>0.0286864</v>
+        <v>0.0016886</v>
       </c>
     </row>
   </sheetData>
@@ -5035,64 +5035,64 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0013344</v>
+        <v>0.026197</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0170352</v>
+        <v>0.0397165</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0476336</v>
+        <v>0.0251423</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0946359</v>
+        <v>0.0432914</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1524476</v>
+        <v>0.0726219</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1768457</v>
+        <v>0.109862</v>
       </c>
       <c r="H2" t="n">
-        <v>0.243637</v>
+        <v>0.1539874</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3255722</v>
+        <v>0.2077264</v>
       </c>
       <c r="J2" t="n">
-        <v>0.4281432</v>
+        <v>0.2692643</v>
       </c>
       <c r="K2" t="n">
-        <v>0.5270932</v>
+        <v>0.3324012</v>
       </c>
       <c r="L2" t="n">
-        <v>0.6425729</v>
+        <v>0.4429099</v>
       </c>
       <c r="M2" t="n">
-        <v>0.771051</v>
+        <v>0.5032802</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9122017</v>
+        <v>0.5781709</v>
       </c>
       <c r="O2" t="n">
-        <v>1.0638718</v>
+        <v>0.6917848</v>
       </c>
       <c r="P2" t="n">
-        <v>1.2445131</v>
+        <v>0.7905346</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.4169654</v>
+        <v>0.91823</v>
       </c>
       <c r="R2" t="n">
-        <v>1.6070893</v>
+        <v>1.0537399</v>
       </c>
       <c r="S2" t="n">
-        <v>1.8183315</v>
+        <v>1.1799597</v>
       </c>
       <c r="T2" t="n">
-        <v>2.010932</v>
+        <v>1.3020939</v>
       </c>
       <c r="U2" t="n">
-        <v>2.2527316</v>
+        <v>1.4397005</v>
       </c>
     </row>
     <row r="3">
@@ -5100,259 +5100,259 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0010239</v>
+        <v>0.0249344</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0118128</v>
+        <v>0.0407635</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0346351</v>
+        <v>0.0318994</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0689649</v>
+        <v>0.027606</v>
       </c>
       <c r="F3" t="n">
-        <v>0.115572</v>
+        <v>0.0467097</v>
       </c>
       <c r="G3" t="n">
-        <v>0.175057</v>
+        <v>0.0685415</v>
       </c>
       <c r="H3" t="n">
-        <v>0.244353</v>
+        <v>0.0962373</v>
       </c>
       <c r="I3" t="n">
-        <v>0.325816</v>
+        <v>0.1300615</v>
       </c>
       <c r="J3" t="n">
-        <v>0.42173</v>
+        <v>0.1641937</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5252814</v>
+        <v>0.2070488</v>
       </c>
       <c r="L3" t="n">
-        <v>0.6444232</v>
+        <v>0.2520725</v>
       </c>
       <c r="M3" t="n">
-        <v>0.7779904</v>
+        <v>0.3328195</v>
       </c>
       <c r="N3" t="n">
-        <v>0.9189178</v>
+        <v>0.3705317</v>
       </c>
       <c r="O3" t="n">
-        <v>1.0693381</v>
+        <v>0.4228309</v>
       </c>
       <c r="P3" t="n">
-        <v>1.2408048</v>
+        <v>0.487505</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.4220621</v>
+        <v>0.5595059</v>
       </c>
       <c r="R3" t="n">
-        <v>1.6167721</v>
+        <v>0.6388389</v>
       </c>
       <c r="S3" t="n">
-        <v>1.8006803</v>
+        <v>0.7249983</v>
       </c>
       <c r="T3" t="n">
-        <v>2.0409709</v>
+        <v>0.802078</v>
       </c>
       <c r="U3" t="n">
-        <v>2.2740962</v>
+        <v>0.8912964</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>8.237E-4</v>
+        <v>0.0055073</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0089051</v>
+        <v>0.0043242</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0252706</v>
+        <v>0.0064389</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0504463</v>
+        <v>0.0090642</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0839677</v>
+        <v>0.0119385</v>
       </c>
       <c r="G4" t="n">
-        <v>0.127467</v>
+        <v>0.0147153</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1834591</v>
+        <v>0.0138684</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2386327</v>
+        <v>0.0101421</v>
       </c>
       <c r="J4" t="n">
-        <v>0.3056447</v>
+        <v>0.0110865</v>
       </c>
       <c r="K4" t="n">
-        <v>0.3852932</v>
+        <v>0.0132268</v>
       </c>
       <c r="L4" t="n">
-        <v>0.4807325</v>
+        <v>0.0139377</v>
       </c>
       <c r="M4" t="n">
-        <v>0.5741725</v>
+        <v>0.0155083</v>
       </c>
       <c r="N4" t="n">
-        <v>0.6685826</v>
+        <v>0.016966</v>
       </c>
       <c r="O4" t="n">
-        <v>0.7798125</v>
+        <v>0.0190062</v>
       </c>
       <c r="P4" t="n">
-        <v>0.8955</v>
+        <v>0.0248369</v>
       </c>
       <c r="Q4" t="n">
-        <v>1.0585133</v>
+        <v>0.0214981</v>
       </c>
       <c r="R4" t="n">
-        <v>1.1853952</v>
+        <v>0.0221038</v>
       </c>
       <c r="S4" t="n">
-        <v>1.3098673</v>
+        <v>0.0246778</v>
       </c>
       <c r="T4" t="n">
-        <v>1.4642859</v>
+        <v>0.0280166</v>
       </c>
       <c r="U4" t="n">
-        <v>1.723421</v>
+        <v>0.0283246</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0035081</v>
+        <v>0.0131319</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0013473</v>
+        <v>0.0102422</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0023892</v>
+        <v>0.0122824</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0034825</v>
+        <v>0.0177667</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0045013</v>
+        <v>0.0145023</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0057254</v>
+        <v>0.0081224</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0070727</v>
+        <v>0.0089795</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0086818</v>
+        <v>0.0106246</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0093876</v>
+        <v>0.0121541</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0104115</v>
+        <v>0.0151182</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0112225</v>
+        <v>0.0211208</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0123106</v>
+        <v>0.0212979</v>
       </c>
       <c r="N5" t="n">
-        <v>0.013332</v>
+        <v>0.0179309</v>
       </c>
       <c r="O5" t="n">
-        <v>0.0151002</v>
+        <v>0.0192166</v>
       </c>
       <c r="P5" t="n">
-        <v>0.0155186</v>
+        <v>0.0209617</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.0169095</v>
+        <v>0.0221602</v>
       </c>
       <c r="R5" t="n">
-        <v>0.0173663</v>
+        <v>0.0242261</v>
       </c>
       <c r="S5" t="n">
-        <v>0.0195272</v>
+        <v>0.0254785</v>
       </c>
       <c r="T5" t="n">
-        <v>0.0202021</v>
+        <v>0.0267411</v>
       </c>
       <c r="U5" t="n">
-        <v>0.0232945</v>
+        <v>0.0281012</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0021813</v>
+        <v>0.0293972</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0018195</v>
+        <v>0.0334495</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0032027</v>
+        <v>0.014297</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0046938</v>
+        <v>0.0285401</v>
       </c>
       <c r="F6" t="n">
-        <v>0.006</v>
+        <v>0.0473128</v>
       </c>
       <c r="G6" t="n">
-        <v>0.007432</v>
+        <v>0.0717751</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0090437</v>
+        <v>0.1030971</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0102858</v>
+        <v>0.1391335</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0116819</v>
+        <v>0.1774231</v>
       </c>
       <c r="K6" t="n">
-        <v>0.0132191</v>
+        <v>0.2246538</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0146126</v>
+        <v>0.2796862</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0161268</v>
+        <v>0.3267681</v>
       </c>
       <c r="N6" t="n">
-        <v>0.0175408</v>
+        <v>0.3812795</v>
       </c>
       <c r="O6" t="n">
-        <v>0.0189318</v>
+        <v>0.4464668</v>
       </c>
       <c r="P6" t="n">
-        <v>0.0204485</v>
+        <v>0.521591</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.0225041</v>
+        <v>0.5894679</v>
       </c>
       <c r="R6" t="n">
-        <v>0.0236564</v>
+        <v>0.6702841</v>
       </c>
       <c r="S6" t="n">
-        <v>0.0251217</v>
+        <v>0.7529635</v>
       </c>
       <c r="T6" t="n">
-        <v>0.0263202</v>
+        <v>0.8378115</v>
       </c>
       <c r="U6" t="n">
-        <v>0.0277317</v>
+        <v>0.9322268</v>
       </c>
     </row>
   </sheetData>
@@ -5438,64 +5438,64 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0020838</v>
+        <v>0.0018477</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0231483</v>
+        <v>0.0206332</v>
       </c>
       <c r="D2" t="n">
-        <v>0.071213</v>
+        <v>0.0598006</v>
       </c>
       <c r="E2" t="n">
-        <v>0.145267</v>
+        <v>0.1197859</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2352656</v>
+        <v>0.1970864</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3185199</v>
+        <v>0.3217586</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4420245</v>
+        <v>0.5365193</v>
       </c>
       <c r="I2" t="n">
-        <v>0.6155879</v>
+        <v>0.6527202</v>
       </c>
       <c r="J2" t="n">
-        <v>0.7621895</v>
+        <v>0.7975612</v>
       </c>
       <c r="K2" t="n">
-        <v>0.9511047</v>
+        <v>0.9894303</v>
       </c>
       <c r="L2" t="n">
-        <v>1.1697252</v>
+        <v>1.1106021</v>
       </c>
       <c r="M2" t="n">
-        <v>1.4088583</v>
+        <v>1.331155</v>
       </c>
       <c r="N2" t="n">
-        <v>1.6697565</v>
+        <v>1.5736166</v>
       </c>
       <c r="O2" t="n">
-        <v>1.96607</v>
+        <v>1.855261</v>
       </c>
       <c r="P2" t="n">
-        <v>2.2645649</v>
+        <v>2.1162465</v>
       </c>
       <c r="Q2" t="n">
-        <v>2.6135575</v>
+        <v>2.4373661</v>
       </c>
       <c r="R2" t="n">
-        <v>2.967616</v>
+        <v>2.7436704</v>
       </c>
       <c r="S2" t="n">
-        <v>3.3865153</v>
+        <v>3.0878818</v>
       </c>
       <c r="T2" t="n">
-        <v>3.7796257</v>
+        <v>3.489982</v>
       </c>
       <c r="U2" t="n">
-        <v>4.1666487</v>
+        <v>3.8955108</v>
       </c>
     </row>
     <row r="3">
@@ -5503,259 +5503,259 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0018169</v>
+        <v>0.001491</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0194784</v>
+        <v>0.0153004</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0576679</v>
+        <v>0.0458757</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1177842</v>
+        <v>0.0976385</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2012156</v>
+        <v>0.167589</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3074128</v>
+        <v>0.260254</v>
       </c>
       <c r="H3" t="n">
-        <v>0.4346566</v>
+        <v>0.3716583</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5847355</v>
+        <v>0.5104249</v>
       </c>
       <c r="J3" t="n">
-        <v>0.7523682</v>
+        <v>0.6693859</v>
       </c>
       <c r="K3" t="n">
-        <v>0.948718</v>
+        <v>0.8478305</v>
       </c>
       <c r="L3" t="n">
-        <v>1.2375302</v>
+        <v>1.0441829</v>
       </c>
       <c r="M3" t="n">
-        <v>1.5109366</v>
+        <v>1.2558461</v>
       </c>
       <c r="N3" t="n">
-        <v>1.8027693</v>
+        <v>1.4808798</v>
       </c>
       <c r="O3" t="n">
-        <v>2.1166494</v>
+        <v>1.7571528</v>
       </c>
       <c r="P3" t="n">
-        <v>2.2792392</v>
+        <v>2.0475433</v>
       </c>
       <c r="Q3" t="n">
-        <v>2.608181</v>
+        <v>2.335896</v>
       </c>
       <c r="R3" t="n">
-        <v>3.3024193</v>
+        <v>2.6136165</v>
       </c>
       <c r="S3" t="n">
-        <v>3.8406966</v>
+        <v>2.955798</v>
       </c>
       <c r="T3" t="n">
-        <v>3.6831907</v>
+        <v>3.3227523</v>
       </c>
       <c r="U3" t="n">
-        <v>4.0803173</v>
+        <v>3.7088514</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>4.952E-4</v>
+        <v>7.237E-4</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0048015</v>
+        <v>0.0027228</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0156905</v>
+        <v>0.0050069</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0260764</v>
+        <v>0.0073679</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0428576</v>
+        <v>0.009734</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0647151</v>
+        <v>0.0123106</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0909096</v>
+        <v>0.0151156</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1204378</v>
+        <v>0.0178385</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1550601</v>
+        <v>0.0200327</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1974816</v>
+        <v>0.0227556</v>
       </c>
       <c r="L4" t="n">
-        <v>0.2495986</v>
+        <v>0.0252347</v>
       </c>
       <c r="M4" t="n">
-        <v>0.2824707</v>
+        <v>0.0278164</v>
       </c>
       <c r="N4" t="n">
-        <v>0.335101</v>
+        <v>0.0302441</v>
       </c>
       <c r="O4" t="n">
-        <v>0.3925483</v>
+        <v>0.0337626</v>
       </c>
       <c r="P4" t="n">
-        <v>0.4499827</v>
+        <v>0.0357951</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.5152496</v>
+        <v>0.0386514</v>
       </c>
       <c r="R4" t="n">
-        <v>0.5873403</v>
+        <v>0.0404222</v>
       </c>
       <c r="S4" t="n">
-        <v>0.6560846</v>
+        <v>0.0451725</v>
       </c>
       <c r="T4" t="n">
-        <v>0.7577036</v>
+        <v>0.0466148</v>
       </c>
       <c r="U4" t="n">
-        <v>0.8275796</v>
+        <v>0.0501306</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>6.929E-4</v>
+        <v>6.159E-4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0026561</v>
+        <v>0.0023456</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0048375</v>
+        <v>0.0042241</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0071395</v>
+        <v>0.0065005</v>
       </c>
       <c r="F5" t="n">
-        <v>0.009462</v>
+        <v>0.0081763</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0119822</v>
+        <v>0.0102576</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0146896</v>
+        <v>0.0127213</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0179694</v>
+        <v>0.0144971</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0196041</v>
+        <v>0.0166118</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0221294</v>
+        <v>0.0188394</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0241902</v>
+        <v>0.0209977</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0277882</v>
+        <v>0.0239053</v>
       </c>
       <c r="N5" t="n">
-        <v>0.029292</v>
+        <v>0.0254374</v>
       </c>
       <c r="O5" t="n">
-        <v>0.0327668</v>
+        <v>0.0276496</v>
       </c>
       <c r="P5" t="n">
-        <v>0.0344632</v>
+        <v>0.029795</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.0374222</v>
+        <v>0.0321484</v>
       </c>
       <c r="R5" t="n">
-        <v>0.0403555</v>
+        <v>0.0343041</v>
       </c>
       <c r="S5" t="n">
-        <v>0.0429475</v>
+        <v>0.0368678</v>
       </c>
       <c r="T5" t="n">
-        <v>0.0448055</v>
+        <v>0.0392494</v>
       </c>
       <c r="U5" t="n">
-        <v>0.0489065</v>
+        <v>0.0425548</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>5.876E-4</v>
+        <v>4.157E-4</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0022814</v>
+        <v>0.0037365</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0041497</v>
+        <v>0.0104424</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0061258</v>
+        <v>0.0206255</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0081429</v>
+        <v>0.0338396</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0101395</v>
+        <v>0.0495789</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0127238</v>
+        <v>0.0699684</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0142816</v>
+        <v>0.0913433</v>
       </c>
       <c r="J6" t="n">
-        <v>0.016386</v>
+        <v>0.1183744</v>
       </c>
       <c r="K6" t="n">
-        <v>0.018747</v>
+        <v>0.1517804</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0208539</v>
+        <v>0.1832307</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0234819</v>
+        <v>0.2207787</v>
       </c>
       <c r="N6" t="n">
-        <v>0.0250525</v>
+        <v>0.2593404</v>
       </c>
       <c r="O6" t="n">
-        <v>0.0273288</v>
+        <v>0.3019517</v>
       </c>
       <c r="P6" t="n">
-        <v>0.0300209</v>
+        <v>0.3472962</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.0320508</v>
+        <v>0.3968802</v>
       </c>
       <c r="R6" t="n">
-        <v>0.0348533</v>
+        <v>0.4521949</v>
       </c>
       <c r="S6" t="n">
-        <v>0.0363982</v>
+        <v>0.5090827</v>
       </c>
       <c r="T6" t="n">
-        <v>0.0385103</v>
+        <v>0.5650697</v>
       </c>
       <c r="U6" t="n">
-        <v>0.041187</v>
+        <v>0.6380151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>